<commit_message>
Implemented code to transfer data to excel sheet
Implemented code in main.py to transfer data obtained from the "Insert
here:" section to the excel spreadsheet

Wrote code to clean the "Insert here:" ection after each entry
</commit_message>
<xml_diff>
--- a/jewel-project.xlsx
+++ b/jewel-project.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Desktop\Repos\Python-Data-Entry-Project-Tkinter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14616ACB-699B-428A-95A8-00F076E7B322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07BFBF1-1385-4B63-A94D-229D62B175E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Type</t>
   </si>
@@ -39,6 +34,18 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Watch</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Sold Out</t>
+  </si>
+  <si>
     <t>Earring</t>
   </si>
   <si>
@@ -49,15 +56,6 @@
   </si>
   <si>
     <t>In Stock</t>
-  </si>
-  <si>
-    <t>Sold out</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Watch</t>
   </si>
 </sst>
 </file>
@@ -387,7 +385,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,16 +421,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -440,6 +438,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>